<commit_message>
change 5v booster --> TPS61022
</commit_message>
<xml_diff>
--- a/doc/Pinout.xlsx
+++ b/doc/Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Private\src\FlightComputer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB5937E-C139-4026-A2FC-DB7C6E6C3512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783AA1EA-317D-4F23-ADC4-FE35EC6165FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="720" windowWidth="25065" windowHeight="13830" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="825" windowWidth="25065" windowHeight="13830" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32F103xx_LQFP48" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="771">
   <si>
     <t>Pins</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2965,6 +2965,10 @@
   </si>
   <si>
     <t>PWR_LED1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPI_STATUS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3400,7 +3404,18 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -5900,8 +5915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7639D5D2-04CD-4D37-AE26-FA795D959713}">
   <dimension ref="B2:M178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8225,8 +8240,8 @@
       <c r="H82" s="25" t="s">
         <v>764</v>
       </c>
-      <c r="I82" s="25" t="s">
-        <v>764</v>
+      <c r="I82" s="41" t="s">
+        <v>770</v>
       </c>
       <c r="J82" s="36" t="s">
         <v>367</v>
@@ -10713,6 +10728,9 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I10:I11">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>